<commit_message>
atualizacao caderno de testes e priorizacao
</commit_message>
<xml_diff>
--- a/Cenarios/Priorização.xlsx
+++ b/Cenarios/Priorização.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24606"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="74" documentId="11_613F185C1EC99B5EEA8E8F5B961B32FB2A73F722" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A565B857-37A5-454A-9E0B-B1639DBE0CD2}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\desafioQA4G5\Cenarios\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1D7727-F4E7-4DB3-ADC6-82993E07FD5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Funcionalidades" sheetId="1" r:id="rId1"/>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
   <si>
     <t>Cod.</t>
   </si>
@@ -111,24 +116,12 @@
     <t>CPF inválido com 10 dígitos</t>
   </si>
   <si>
-    <t>CPF válido com 11 dígitos</t>
-  </si>
-  <si>
-    <t>E-mail com domínio inválido</t>
-  </si>
-  <si>
-    <t>E-mail válido</t>
-  </si>
-  <si>
     <t>Senha com &lt; 5 caracteres</t>
   </si>
   <si>
     <t>Senha com 5 caracteres</t>
   </si>
   <si>
-    <t>Validar resultado de Endereço a partir do CEP inserido</t>
-  </si>
-  <si>
     <t>Adicionar cupom de desconto inválido</t>
   </si>
   <si>
@@ -154,13 +147,25 @@
   </si>
   <si>
     <t>E-mail inválido e senha válida</t>
+  </si>
+  <si>
+    <t>E-mail  inválido</t>
+  </si>
+  <si>
+    <t>Dados válidos e validação</t>
+  </si>
+  <si>
+    <t>Data de nascimento inválida</t>
+  </si>
+  <si>
+    <t>BAIXA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +185,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -240,10 +252,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -257,9 +270,12 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -275,7 +291,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -577,13 +593,13 @@
       <selection activeCell="C8" sqref="C8:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5">
+    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,7 +610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="3:5">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="2">
         <v>1</v>
       </c>
@@ -605,7 +621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="3:5">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C5" s="3">
         <v>2</v>
       </c>
@@ -616,7 +632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:5">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C6" s="2">
         <v>3</v>
       </c>
@@ -627,7 +643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:5">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C7" s="3">
         <v>4</v>
       </c>
@@ -638,7 +654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="3:5">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C8" s="2">
         <v>5</v>
       </c>
@@ -649,7 +665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="3:5">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C9" s="3">
         <v>6</v>
       </c>
@@ -660,7 +676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="3:5">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C10" s="2">
         <v>7</v>
       </c>
@@ -671,7 +687,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="3:5">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>8</v>
       </c>
@@ -682,7 +698,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="3:5">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" s="4">
         <v>9</v>
       </c>
@@ -703,18 +719,18 @@
   <dimension ref="B2:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C5"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -734,7 +750,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -755,7 +771,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -776,7 +792,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>3</v>
       </c>
@@ -797,7 +813,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -818,44 +834,109 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="2:7">
+      <c r="D7" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="E7" s="10">
+        <v>3</v>
+      </c>
+      <c r="F7" s="10">
+        <f>D7*E7</f>
+        <v>2.0999999999999996</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="2:7">
+      <c r="D8" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="E8" s="7">
+        <v>3</v>
+      </c>
+      <c r="F8" s="7">
+        <f>D8*E8</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="2:7">
+      <c r="D9" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="E9" s="10">
+        <v>1</v>
+      </c>
+      <c r="F9" s="10">
+        <f>D9*E9</f>
+        <v>0.6</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="2:7">
+      <c r="D10" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7">
+        <f>D10*E10</f>
+        <v>0.6</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0.65</v>
+      </c>
+      <c r="E11" s="14">
+        <v>1</v>
+      </c>
+      <c r="F11" s="14">
+        <f>D11*E11</f>
+        <v>0.65</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -865,23 +946,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{284DE2E4-3998-4075-A881-48D6E4452992}">
-  <dimension ref="A2:B26"/>
+  <dimension ref="A2:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -889,7 +970,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -897,7 +978,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -905,7 +986,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -913,7 +994,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -921,12 +1002,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" s="12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -934,134 +1015,126 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>12</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="B16" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>16</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="B21" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="B21" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>18</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>20</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26">
-        <v>21</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1070,21 +1143,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010092F429CBFAA7374CB672B486FF605DE7" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="41366addc85771bf794e97adbfef3340">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4305ba7b-0145-46eb-bee1-47fa612a8471" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ef3c72b46829ba03409bc947caebf836" ns2:_="">
     <xsd:import namespace="4305ba7b-0145-46eb-bee1-47fa612a8471"/>
@@ -1216,14 +1274,52 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4C678E1-AFE1-43CB-8112-BCA6CD78A92C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C45D5988-9F02-48B2-9EF2-7B48EEC69392}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4305ba7b-0145-46eb-bee1-47fa612a8471"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73C5299E-64F6-4AE9-8A53-A914B1117B22}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73C5299E-64F6-4AE9-8A53-A914B1117B22}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C45D5988-9F02-48B2-9EF2-7B48EEC69392}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4C678E1-AFE1-43CB-8112-BCA6CD78A92C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>